<commit_message>
Added Final Design Review
Also added weekly activity report
</commit_message>
<xml_diff>
--- a/Content/WBS.xlsx
+++ b/Content/WBS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\7-Fall-2019\BluSh3ll\Assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\7-Fall-2019\BluSh3ll\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D649C2-707E-417A-A6D1-E4F89CE09E4A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCC776E-271F-486D-B9F5-79472F4EC99D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="104">
   <si>
     <t>ID</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Customer Deployment</t>
   </si>
   <si>
-    <t>Findal Development</t>
-  </si>
-  <si>
     <t>Final touches and packaging and workflow to meet customer requests.</t>
   </si>
   <si>
@@ -296,7 +293,58 @@
     <t>Mitch Palmer</t>
   </si>
   <si>
-    <t>Carl Bai</t>
+    <t>Total Hours</t>
+  </si>
+  <si>
+    <t>Carl</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>Final Development</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
@@ -333,7 +381,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,11 +412,105 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -377,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -406,42 +548,99 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,79 +746,76 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Team Hours'!$B$1:$Y$1</c:f>
+              <c:f>'Team Hours'!$B$1:$X$1</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>Wk4</c:v>
+                  <c:v>Wk5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Wk5</c:v>
+                  <c:v>Wk6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Wk6</c:v>
+                  <c:v>Wk7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Wk7</c:v>
+                  <c:v>Wk8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Wk8</c:v>
+                  <c:v>Wk9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Wk9</c:v>
+                  <c:v>Wk10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Wk10</c:v>
+                  <c:v>Wk11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Wk11</c:v>
+                  <c:v>Wk12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Wk12</c:v>
+                  <c:v>Wk13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Wk13</c:v>
+                  <c:v>Wk14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Wk14</c:v>
+                  <c:v>Wk15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Wk15</c:v>
+                  <c:v>Wk16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Wk16</c:v>
+                  <c:v>Wk17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Wk17</c:v>
+                  <c:v>Wk18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Wk18</c:v>
+                  <c:v>Wk19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Wk19</c:v>
+                  <c:v>Wk20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Wk20</c:v>
+                  <c:v>Wk21</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Wk21</c:v>
+                  <c:v>Wk22</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Wk22</c:v>
+                  <c:v>Wk23</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Wk23</c:v>
+                  <c:v>Wk24</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Wk24</c:v>
+                  <c:v>Wk25</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Wk25</c:v>
+                  <c:v>Wk26</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Wk26</c:v>
-                </c:pt>
-                <c:pt idx="23">
                   <c:v>Wk27</c:v>
                 </c:pt>
               </c:strCache>
@@ -627,10 +823,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Team Hours'!$B$7:$Y$7</c:f>
+              <c:f>'Team Hours'!$B$7:$X$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>11</c:v>
                 </c:pt>
@@ -638,70 +834,25 @@
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>36</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -884,7 +1035,456 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Team Hours'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Hours</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Team Hours'!$B$1:$X$1</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>Wk5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Wk6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Wk7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wk8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Wk9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Wk10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Wk11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Wk12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Wk13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Wk14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Wk15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Wk16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Wk17</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Wk18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Wk19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Wk20</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Wk21</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Wk22</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Wk23</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Wk24</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Wk25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Wk26</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Wk27</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Team Hours'!$B$8:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1BC6-414C-9AC5-4AA900635DE6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="797596784"/>
+        <c:axId val="797598424"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="797596784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="797598424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="797598424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="797596784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1440,20 +2040,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>300129</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>35111</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>87218</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>35112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>268941</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>89646</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>347382</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1475,6 +2591,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>386601</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>34739</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>67235</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>145678</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C9FF13E-A5F5-4A30-A3D2-7D90DC6EDF0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1749,12 +2901,12 @@
   <dimension ref="A1:AI18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="1" bestFit="1" customWidth="1"/>
@@ -1798,7 +2950,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" s="8">
         <v>43703</v>
@@ -1841,7 +2993,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="9">
         <v>43745</v>
@@ -1861,10 +3013,10 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="9">
         <v>43752</v>
@@ -1884,10 +3036,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="9">
         <v>43759</v>
@@ -1907,7 +3059,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="8">
         <v>43766</v>
@@ -1927,12 +3079,12 @@
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="12">
+        <v>72</v>
+      </c>
+      <c r="E8" s="10">
         <v>43766</v>
       </c>
       <c r="F8" s="9">
@@ -1950,15 +3102,15 @@
         <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" s="9">
         <v>43780</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="10">
         <v>43793</v>
       </c>
       <c r="G9" s="1">
@@ -1973,12 +3125,12 @@
         <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="12">
+        <v>75</v>
+      </c>
+      <c r="E10" s="10">
         <v>43794</v>
       </c>
       <c r="F10" s="9">
@@ -1996,15 +3148,15 @@
         <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>78</v>
+        <v>35</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>77</v>
       </c>
       <c r="E11" s="9">
         <v>43485</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="10">
         <v>43498</v>
       </c>
       <c r="G11" s="1">
@@ -2019,10 +3171,10 @@
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="12">
+        <v>36</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="10">
         <v>43499</v>
       </c>
       <c r="F12" s="9">
@@ -2040,9 +3192,9 @@
         <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="18"/>
+        <v>37</v>
+      </c>
+      <c r="D13" s="16"/>
       <c r="E13" s="8">
         <v>43513</v>
       </c>
@@ -2061,13 +3213,13 @@
         <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="12">
+        <v>38</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="10">
         <v>43513</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="10">
         <v>43519</v>
       </c>
       <c r="G14" s="1">
@@ -2082,10 +3234,10 @@
         <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="12">
+        <v>39</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="10">
         <v>43520</v>
       </c>
       <c r="F15" s="9">
@@ -2103,9 +3255,9 @@
         <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="18"/>
+        <v>40</v>
+      </c>
+      <c r="D16" s="16"/>
       <c r="E16" s="9">
         <v>43526</v>
       </c>
@@ -2124,13 +3276,13 @@
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="18"/>
+        <v>41</v>
+      </c>
+      <c r="D17" s="16"/>
       <c r="E17" s="9">
         <v>43540</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="10">
         <v>43546</v>
       </c>
       <c r="G17" s="1">
@@ -2142,13 +3294,13 @@
         <v>4.5</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="12">
+      <c r="D18" s="16"/>
+      <c r="E18" s="10">
         <v>43547</v>
       </c>
       <c r="F18" s="9">
@@ -2170,643 +3322,811 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF51B197-A615-4074-96E4-CE4CCB37617D}">
-  <dimension ref="A1:AB24"/>
+  <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:AB1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="28" width="5.85546875" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="4" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="5.85546875" customWidth="1"/>
+    <col min="11" max="14" width="5.85546875" style="17" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="40" customWidth="1"/>
+    <col min="16" max="17" width="5.85546875" customWidth="1"/>
+    <col min="18" max="18" width="5.85546875" style="40" customWidth="1"/>
+    <col min="19" max="24" width="5.85546875" customWidth="1"/>
+    <col min="25" max="25" width="5.85546875" style="44" customWidth="1"/>
+    <col min="26" max="29" width="5.85546875" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="P1" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="S1" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="Z1" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AA1" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AB1" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AC1" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="AB1" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="19" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="19" t="s">
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
+      <c r="AB3" s="18"/>
+      <c r="AC3" s="18"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="25">
+        <v>2.1</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="26">
+        <v>2.1</v>
+      </c>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="26">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="18"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="26">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="18"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="19">
+        <v>3</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="P7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="S7" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z7" s="18"/>
+      <c r="AA7" s="18"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="18"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="25">
+        <v>3.1</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="34">
+        <v>3.1</v>
+      </c>
+      <c r="L8" s="35"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="18"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="25">
+        <v>3.2</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="34">
+        <v>3.2</v>
+      </c>
+      <c r="N9" s="35"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z9" s="18"/>
+      <c r="AA9" s="18"/>
+      <c r="AB9" s="18"/>
+      <c r="AC9" s="18"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="25">
+        <v>3.3</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="P10" s="34">
+        <v>3.3</v>
+      </c>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="43"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="18"/>
+      <c r="AC10" s="18"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="25">
+        <v>3.4</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="S11" s="34">
+        <v>3.4</v>
+      </c>
+      <c r="T11" s="35"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="18"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z11" s="18"/>
+      <c r="AA11" s="18"/>
+      <c r="AB11" s="18"/>
+      <c r="AC11" s="18"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="25">
+        <v>3.5</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="S12" s="18"/>
+      <c r="T12" s="18"/>
+      <c r="U12" s="36">
+        <v>3.5</v>
+      </c>
+      <c r="V12" s="37"/>
+      <c r="W12" s="18"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z12" s="18"/>
+      <c r="AA12" s="18"/>
+      <c r="AB12" s="18"/>
+      <c r="AC12" s="18"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="19">
+        <v>4</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="X13" s="24"/>
+      <c r="Y13" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z13" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="S7" s="20"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="20"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="W13" s="20"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z13" s="19"/>
-      <c r="AA13" s="19"/>
-      <c r="AB13" s="19"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="14"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="10"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="14"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="10"/>
-      <c r="AB18" s="10"/>
-    </row>
-    <row r="19" spans="1:28" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:28" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:28" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:28" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:28" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.25"/>
+      <c r="AA13" s="23"/>
+      <c r="AB13" s="23"/>
+      <c r="AC13" s="23"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
+      <c r="W14" s="26">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z14" s="18"/>
+      <c r="AA14" s="18"/>
+      <c r="AB14" s="18"/>
+      <c r="AC14" s="18"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="25">
+        <v>4.2</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="42">
+        <v>4.2</v>
+      </c>
+      <c r="Y15" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z15" s="18"/>
+      <c r="AA15" s="18"/>
+      <c r="AB15" s="18"/>
+      <c r="AC15" s="18"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="25">
+        <v>4.3</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="18"/>
+      <c r="U16" s="18"/>
+      <c r="V16" s="18"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="43"/>
+      <c r="Z16" s="29">
+        <v>4.2</v>
+      </c>
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="18"/>
+      <c r="AC16" s="18"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17" s="25">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
+      <c r="U17" s="18"/>
+      <c r="V17" s="18"/>
+      <c r="W17" s="18"/>
+      <c r="X17" s="18"/>
+      <c r="Y17" s="43"/>
+      <c r="Z17" s="18"/>
+      <c r="AA17" s="26">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AB17" s="18"/>
+      <c r="AC17" s="18"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A18" s="25">
+        <v>4.5</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="18"/>
+      <c r="U18" s="18"/>
+      <c r="V18" s="18"/>
+      <c r="W18" s="18"/>
+      <c r="X18" s="18"/>
+      <c r="Y18" s="43"/>
+      <c r="Z18" s="18"/>
+      <c r="AA18" s="18"/>
+      <c r="AB18" s="34">
+        <v>4.5</v>
+      </c>
+      <c r="AC18" s="35"/>
+    </row>
+    <row r="19" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="33" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="34" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="35" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="36" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="Y13:AB13"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="R7:U7"/>
-    <mergeCell ref="O7:P7"/>
+  <mergeCells count="13">
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="Z13:AC13"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="S7:V7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="U12:V12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2817,13 +4137,16 @@
   <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="25" width="5.85546875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="5" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="24" width="5.85546875" style="11" customWidth="1"/>
+    <col min="25" max="25" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -2854,14 +4177,14 @@
       <c r="J1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="4" t="s">
         <v>56</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>60</v>
@@ -2881,10 +4204,10 @@
       <c r="S1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="U1" s="4" t="s">
         <v>67</v>
       </c>
       <c r="V1" s="4" t="s">
@@ -2896,498 +4219,335 @@
       <c r="X1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="Y1" s="4" t="s">
-        <v>71</v>
+      <c r="Y1" s="15" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="15">
+        <v>82</v>
+      </c>
+      <c r="B2" s="14">
         <v>4</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="14">
         <v>7</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
+        <v>9</v>
+      </c>
+      <c r="E2" s="14">
+        <v>7</v>
+      </c>
+      <c r="F2" s="14">
         <v>6</v>
       </c>
-      <c r="E2" s="15">
-        <v>4</v>
-      </c>
-      <c r="F2" s="15">
-        <v>4</v>
-      </c>
-      <c r="G2" s="15">
-        <v>4</v>
-      </c>
-      <c r="H2" s="15">
-        <v>12</v>
-      </c>
-      <c r="I2" s="15">
-        <v>12</v>
-      </c>
-      <c r="J2" s="15">
-        <v>12</v>
-      </c>
-      <c r="K2" s="15">
-        <v>12</v>
-      </c>
-      <c r="L2" s="15">
-        <v>0</v>
-      </c>
-      <c r="M2" s="15">
-        <v>24</v>
-      </c>
-      <c r="N2" s="15">
-        <v>24</v>
-      </c>
-      <c r="O2" s="15">
-        <v>12</v>
-      </c>
-      <c r="P2" s="15">
-        <v>12</v>
-      </c>
-      <c r="Q2" s="15">
-        <v>12</v>
-      </c>
-      <c r="R2" s="15">
-        <v>12</v>
-      </c>
-      <c r="S2" s="15">
-        <v>6</v>
-      </c>
-      <c r="T2" s="15">
-        <v>6</v>
-      </c>
-      <c r="U2" s="15">
-        <v>0</v>
-      </c>
-      <c r="V2" s="15">
-        <v>0</v>
-      </c>
-      <c r="W2" s="15">
-        <v>0</v>
-      </c>
-      <c r="X2" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="15">
-        <v>0</v>
+      <c r="G2" s="14">
+        <v>7</v>
+      </c>
+      <c r="H2" s="14">
+        <v>5</v>
+      </c>
+      <c r="I2" s="14">
+        <v>5</v>
+      </c>
+      <c r="J2" s="14">
+        <v>8</v>
+      </c>
+      <c r="Y2">
+        <f>AVERAGE(B2:X2)</f>
+        <v>6.4444444444444446</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="15">
+        <v>83</v>
+      </c>
+      <c r="B3" s="14">
         <v>3</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>8</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
+        <v>7</v>
+      </c>
+      <c r="E3" s="14">
+        <v>7</v>
+      </c>
+      <c r="F3" s="14">
         <v>6</v>
       </c>
-      <c r="E3" s="15">
+      <c r="G3" s="14">
         <v>6</v>
       </c>
-      <c r="F3" s="15">
+      <c r="H3" s="14">
         <v>6</v>
       </c>
-      <c r="G3" s="15">
+      <c r="I3" s="14">
         <v>6</v>
       </c>
-      <c r="H3" s="15">
-        <v>6</v>
-      </c>
-      <c r="I3" s="15">
-        <v>6</v>
-      </c>
-      <c r="J3" s="15">
-        <v>6</v>
-      </c>
-      <c r="K3" s="15">
-        <v>6</v>
-      </c>
-      <c r="L3" s="15">
-        <v>0</v>
-      </c>
-      <c r="M3" s="15">
-        <v>6</v>
-      </c>
-      <c r="N3" s="15">
-        <v>6</v>
-      </c>
-      <c r="O3" s="15">
-        <v>6</v>
-      </c>
-      <c r="P3" s="15">
-        <v>6</v>
-      </c>
-      <c r="Q3" s="15">
-        <v>6</v>
-      </c>
-      <c r="R3" s="15">
-        <v>6</v>
-      </c>
-      <c r="S3" s="15">
-        <v>6</v>
-      </c>
-      <c r="T3" s="15">
-        <v>6</v>
-      </c>
-      <c r="U3" s="15">
-        <v>0</v>
-      </c>
-      <c r="V3" s="15">
-        <v>6</v>
-      </c>
-      <c r="W3" s="15">
-        <v>6</v>
-      </c>
-      <c r="X3" s="15">
-        <v>6</v>
-      </c>
-      <c r="Y3" s="15">
-        <v>6</v>
+      <c r="J3" s="14">
+        <v>8</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ref="Y3:Y7" si="0">AVERAGE(B3:X3)</f>
+        <v>6.333333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="15">
+        <v>84</v>
+      </c>
+      <c r="B4" s="14">
         <v>2</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>9</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
+        <v>8</v>
+      </c>
+      <c r="E4" s="14">
+        <v>5</v>
+      </c>
+      <c r="F4" s="14">
         <v>6</v>
       </c>
-      <c r="E4" s="15">
+      <c r="G4" s="14">
+        <v>7</v>
+      </c>
+      <c r="H4" s="14">
+        <v>7</v>
+      </c>
+      <c r="I4" s="14">
         <v>6</v>
       </c>
-      <c r="F4" s="15">
-        <v>6</v>
-      </c>
-      <c r="G4" s="15">
-        <v>6</v>
-      </c>
-      <c r="H4" s="15">
-        <v>6</v>
-      </c>
-      <c r="I4" s="15">
-        <v>6</v>
-      </c>
-      <c r="J4" s="15">
-        <v>6</v>
-      </c>
-      <c r="K4" s="15">
-        <v>6</v>
-      </c>
-      <c r="L4" s="15">
-        <v>0</v>
-      </c>
-      <c r="M4" s="15">
-        <v>6</v>
-      </c>
-      <c r="N4" s="15">
-        <v>6</v>
-      </c>
-      <c r="O4" s="15">
-        <v>6</v>
-      </c>
-      <c r="P4" s="15">
-        <v>6</v>
-      </c>
-      <c r="Q4" s="15">
-        <v>6</v>
-      </c>
-      <c r="R4" s="15">
-        <v>6</v>
-      </c>
-      <c r="S4" s="15">
-        <v>6</v>
-      </c>
-      <c r="T4" s="15">
-        <v>6</v>
-      </c>
-      <c r="U4" s="15">
-        <v>0</v>
-      </c>
-      <c r="V4" s="15">
-        <v>6</v>
-      </c>
-      <c r="W4" s="15">
-        <v>6</v>
-      </c>
-      <c r="X4" s="15">
-        <v>6</v>
-      </c>
-      <c r="Y4" s="15">
-        <v>6</v>
+      <c r="J4" s="14">
+        <v>7</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="0"/>
+        <v>6.333333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="15">
+        <v>85</v>
+      </c>
+      <c r="B5" s="14">
         <v>1</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>9</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
+        <v>8</v>
+      </c>
+      <c r="E5" s="14">
+        <v>5</v>
+      </c>
+      <c r="F5" s="14">
         <v>6</v>
       </c>
-      <c r="E5" s="15">
-        <v>6</v>
-      </c>
-      <c r="F5" s="15">
-        <v>6</v>
-      </c>
-      <c r="G5" s="15">
-        <v>6</v>
-      </c>
-      <c r="H5" s="15">
-        <v>6</v>
-      </c>
-      <c r="I5" s="15">
-        <v>6</v>
-      </c>
-      <c r="J5" s="15">
-        <v>6</v>
-      </c>
-      <c r="K5" s="15">
-        <v>6</v>
-      </c>
-      <c r="L5" s="15">
-        <v>0</v>
-      </c>
-      <c r="M5" s="15">
-        <v>6</v>
-      </c>
-      <c r="N5" s="15">
-        <v>6</v>
-      </c>
-      <c r="O5" s="15">
-        <v>6</v>
-      </c>
-      <c r="P5" s="15">
-        <v>6</v>
-      </c>
-      <c r="Q5" s="15">
-        <v>6</v>
-      </c>
-      <c r="R5" s="15">
-        <v>6</v>
-      </c>
-      <c r="S5" s="15">
-        <v>6</v>
-      </c>
-      <c r="T5" s="15">
-        <v>6</v>
-      </c>
-      <c r="U5" s="15">
-        <v>0</v>
-      </c>
-      <c r="V5" s="15">
-        <v>6</v>
-      </c>
-      <c r="W5" s="15">
-        <v>6</v>
-      </c>
-      <c r="X5" s="15">
-        <v>6</v>
-      </c>
-      <c r="Y5" s="15">
-        <v>6</v>
+      <c r="G5" s="14">
+        <v>7</v>
+      </c>
+      <c r="H5" s="14">
+        <v>8</v>
+      </c>
+      <c r="I5" s="14">
+        <v>5</v>
+      </c>
+      <c r="J5" s="14">
+        <v>8</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="0"/>
+        <v>6.333333333333333</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>8</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
+        <v>9</v>
+      </c>
+      <c r="E6" s="14">
+        <v>7</v>
+      </c>
+      <c r="F6" s="14">
         <v>6</v>
       </c>
-      <c r="E6" s="15">
+      <c r="G6" s="14">
         <v>6</v>
       </c>
-      <c r="F6" s="15">
+      <c r="H6" s="14">
+        <v>7</v>
+      </c>
+      <c r="I6" s="14">
         <v>6</v>
       </c>
-      <c r="G6" s="15">
-        <v>6</v>
-      </c>
-      <c r="H6" s="15">
-        <v>6</v>
-      </c>
-      <c r="I6" s="15">
-        <v>6</v>
-      </c>
-      <c r="J6" s="15">
-        <v>6</v>
-      </c>
-      <c r="K6" s="15">
-        <v>6</v>
-      </c>
-      <c r="L6" s="15">
-        <v>0</v>
-      </c>
-      <c r="M6" s="15">
-        <v>6</v>
-      </c>
-      <c r="N6" s="15">
-        <v>6</v>
-      </c>
-      <c r="O6" s="15">
-        <v>6</v>
-      </c>
-      <c r="P6" s="15">
-        <v>6</v>
-      </c>
-      <c r="Q6" s="15">
-        <v>6</v>
-      </c>
-      <c r="R6" s="15">
-        <v>6</v>
-      </c>
-      <c r="S6" s="15">
-        <v>6</v>
-      </c>
-      <c r="T6" s="15">
-        <v>6</v>
-      </c>
-      <c r="U6" s="15">
-        <v>0</v>
-      </c>
-      <c r="V6" s="15">
-        <v>6</v>
-      </c>
-      <c r="W6" s="15">
-        <v>6</v>
-      </c>
-      <c r="X6" s="15">
-        <v>6</v>
-      </c>
-      <c r="Y6" s="15">
-        <v>6</v>
+      <c r="J6" s="14">
+        <v>9</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="0"/>
+        <v>6.5555555555555554</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="15">
-        <f>SUM(B2:B6)</f>
+        <v>81</v>
+      </c>
+      <c r="B7" s="14">
+        <f t="shared" ref="B7:J7" si="1">SUM(B2:B6)</f>
         <v>11</v>
       </c>
-      <c r="C7" s="15">
-        <f t="shared" ref="C7:Y7" si="0">SUM(C2:C6)</f>
+      <c r="C7" s="14">
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="Y7">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="E7" s="15">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="F7" s="15">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="G7" s="15">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="H7" s="15">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="I7" s="15">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="J7" s="15">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="K7" s="15">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="L7" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="15">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="N7" s="15">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="O7" s="15">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="P7" s="15">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="Q7" s="15">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="R7" s="15">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="S7" s="15">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="T7" s="15">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="U7" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V7" s="15">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="W7" s="15">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="X7" s="15">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="Y7" s="15">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="11">
+        <f>B7</f>
+        <v>11</v>
+      </c>
+      <c r="C8" s="12">
+        <f>B8+C7</f>
+        <v>52</v>
+      </c>
+      <c r="D8" s="12">
+        <f t="shared" ref="D8:X8" si="2">C8+D7</f>
+        <v>93</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="G8" s="12">
+        <f t="shared" si="2"/>
+        <v>187</v>
+      </c>
+      <c r="H8" s="12">
+        <f t="shared" si="2"/>
+        <v>220</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" si="2"/>
+        <v>248</v>
+      </c>
+      <c r="J8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="K8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="L8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="M8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="N8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="O8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="P8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="Q8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="R8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="S8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="T8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="U8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="V8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="W8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="X8" s="12">
+        <f t="shared" si="2"/>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="A13" s="11"/>
+      <c r="L13"/>
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13"/>
@@ -3400,10 +4560,10 @@
       <c r="V13"/>
       <c r="W13"/>
       <c r="X13"/>
-      <c r="Y13"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A14" s="11"/>
+      <c r="L14"/>
       <c r="M14"/>
       <c r="N14"/>
       <c r="O14"/>
@@ -3416,10 +4576,10 @@
       <c r="V14"/>
       <c r="W14"/>
       <c r="X14"/>
-      <c r="Y14"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="A15" s="11"/>
+      <c r="L15"/>
       <c r="M15"/>
       <c r="N15"/>
       <c r="O15"/>
@@ -3432,10 +4592,10 @@
       <c r="V15"/>
       <c r="W15"/>
       <c r="X15"/>
-      <c r="Y15"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
+      <c r="A16" s="11"/>
+      <c r="L16"/>
       <c r="M16"/>
       <c r="N16"/>
       <c r="O16"/>
@@ -3448,10 +4608,10 @@
       <c r="V16"/>
       <c r="W16"/>
       <c r="X16"/>
-      <c r="Y16"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="L17"/>
       <c r="M17"/>
       <c r="N17"/>
       <c r="O17"/>
@@ -3464,10 +4624,10 @@
       <c r="V17"/>
       <c r="W17"/>
       <c r="X17"/>
-      <c r="Y17"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="L18"/>
       <c r="M18"/>
       <c r="N18"/>
       <c r="O18"/>
@@ -3480,10 +4640,10 @@
       <c r="V18"/>
       <c r="W18"/>
       <c r="X18"/>
-      <c r="Y18"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="L19"/>
       <c r="M19"/>
       <c r="N19"/>
       <c r="O19"/>
@@ -3496,10 +4656,10 @@
       <c r="V19"/>
       <c r="W19"/>
       <c r="X19"/>
-      <c r="Y19"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="L20"/>
       <c r="M20"/>
       <c r="N20"/>
       <c r="O20"/>
@@ -3512,10 +4672,10 @@
       <c r="V20"/>
       <c r="W20"/>
       <c r="X20"/>
-      <c r="Y20"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="L21"/>
       <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
@@ -3528,10 +4688,10 @@
       <c r="V21"/>
       <c r="W21"/>
       <c r="X21"/>
-      <c r="Y21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Moved Assignments to folder for last semester.
</commit_message>
<xml_diff>
--- a/Content/WBS.xlsx
+++ b/Content/WBS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\7-Fall-2019\BluSh3ll\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BluSh3ll\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCC776E-271F-486D-B9F5-79472F4EC99D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6F7C5C-A475-4C23-B705-2D2674A9F193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -519,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -583,12 +585,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -614,18 +610,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -641,6 +625,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,9 +751,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Team Hours'!$B$1:$X$1</c:f>
+              <c:f>'Team Hours'!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>Wk5</c:v>
                 </c:pt>
@@ -814,19 +819,16 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>Wk26</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Wk27</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Team Hours'!$B$7:$X$7</c:f>
+              <c:f>'Team Hours'!$B$7:$W$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>11</c:v>
                 </c:pt>
@@ -853,6 +855,45 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1113,9 +1154,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Team Hours'!$B$1:$X$1</c:f>
+              <c:f>'Team Hours'!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>Wk5</c:v>
                 </c:pt>
@@ -1181,19 +1222,16 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>Wk26</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Wk27</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Team Hours'!$B$8:$X$8</c:f>
+              <c:f>'Team Hours'!$B$8:$W$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>11</c:v>
                 </c:pt>
@@ -1225,43 +1263,40 @@
                   <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>288</c:v>
+                  <c:v>321</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>288</c:v>
+                  <c:v>356</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>288</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>288</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>288</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>288</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>288</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>288</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>288</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>288</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>288</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>288</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>288</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2604,7 +2639,7 @@
       <xdr:rowOff>34739</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>67235</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>145678</xdr:rowOff>
@@ -3150,7 +3185,7 @@
       <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="39" t="s">
         <v>77</v>
       </c>
       <c r="E11" s="9">
@@ -3173,7 +3208,7 @@
       <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="16"/>
+      <c r="D12" s="39"/>
       <c r="E12" s="10">
         <v>43499</v>
       </c>
@@ -3194,7 +3229,7 @@
       <c r="C13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="8">
         <v>43513</v>
       </c>
@@ -3215,7 +3250,7 @@
       <c r="C14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="10">
         <v>43513</v>
       </c>
@@ -3236,7 +3271,7 @@
       <c r="C15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="16"/>
+      <c r="D15" s="39"/>
       <c r="E15" s="10">
         <v>43520</v>
       </c>
@@ -3257,7 +3292,7 @@
       <c r="C16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="39"/>
       <c r="E16" s="9">
         <v>43526</v>
       </c>
@@ -3278,7 +3313,7 @@
       <c r="C17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="16"/>
+      <c r="D17" s="39"/>
       <c r="E17" s="9">
         <v>43540</v>
       </c>
@@ -3299,7 +3334,7 @@
       <c r="C18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="39"/>
       <c r="E18" s="10">
         <v>43547</v>
       </c>
@@ -3322,46 +3357,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF51B197-A615-4074-96E4-CE4CCB37617D}">
-  <dimension ref="A1:AC36"/>
+  <dimension ref="A1:AC42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" style="23" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="5.85546875" customWidth="1"/>
     <col min="11" max="14" width="5.85546875" style="17" customWidth="1"/>
-    <col min="15" max="15" width="5.85546875" style="40" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="34" customWidth="1"/>
     <col min="16" max="17" width="5.85546875" customWidth="1"/>
-    <col min="18" max="18" width="5.85546875" style="40" customWidth="1"/>
+    <col min="18" max="18" width="5.85546875" style="34" customWidth="1"/>
     <col min="19" max="24" width="5.85546875" customWidth="1"/>
-    <col min="25" max="25" width="5.85546875" style="44" customWidth="1"/>
+    <col min="25" max="25" width="5.85546875" style="38" customWidth="1"/>
     <col min="26" max="29" width="5.85546875" customWidth="1"/>
     <col min="30" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="29" t="s">
         <v>47</v>
       </c>
       <c r="H1" s="19" t="s">
@@ -3382,22 +3417,22 @@
       <c r="M1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="25" t="s">
         <v>54</v>
       </c>
       <c r="O1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="P1" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="Q1" s="25" t="s">
         <v>59</v>
       </c>
       <c r="R1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="S1" s="26" t="s">
         <v>60</v>
       </c>
       <c r="T1" s="19" t="s">
@@ -3412,13 +3447,13 @@
       <c r="W1" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="X1" s="25" t="s">
         <v>65</v>
       </c>
       <c r="Y1" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="Z1" s="28" t="s">
+      <c r="Z1" s="26" t="s">
         <v>67</v>
       </c>
       <c r="AA1" s="19" t="s">
@@ -3435,14 +3470,14 @@
       <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
@@ -3450,17 +3485,17 @@
       <c r="L2" s="18"/>
       <c r="M2" s="18"/>
       <c r="N2" s="18"/>
-      <c r="O2" s="38"/>
+      <c r="O2" s="32"/>
       <c r="P2" s="18"/>
       <c r="Q2" s="18"/>
-      <c r="R2" s="41"/>
+      <c r="R2" s="35"/>
       <c r="S2" s="18"/>
       <c r="T2" s="18"/>
       <c r="U2" s="18"/>
       <c r="V2" s="18"/>
       <c r="W2" s="18"/>
       <c r="X2" s="18"/>
-      <c r="Y2" s="43"/>
+      <c r="Y2" s="37"/>
       <c r="Z2" s="18"/>
       <c r="AA2" s="18"/>
       <c r="AB2" s="18"/>
@@ -3476,33 +3511,33 @@
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
-      <c r="O3" s="38"/>
+      <c r="O3" s="32"/>
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
-      <c r="R3" s="41"/>
+      <c r="R3" s="35"/>
       <c r="S3" s="18"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
       <c r="V3" s="18"/>
       <c r="W3" s="18"/>
       <c r="X3" s="18"/>
-      <c r="Y3" s="43"/>
+      <c r="Y3" s="37"/>
       <c r="Z3" s="18"/>
       <c r="AA3" s="18"/>
       <c r="AB3" s="18"/>
       <c r="AC3" s="18"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="25">
+      <c r="A4" s="23">
         <v>2.1</v>
       </c>
       <c r="B4" s="18"/>
@@ -3511,7 +3546,7 @@
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="26">
+      <c r="H4" s="24">
         <v>2.1</v>
       </c>
       <c r="I4" s="18"/>
@@ -3520,10 +3555,10 @@
       <c r="L4" s="18"/>
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
-      <c r="O4" s="39"/>
+      <c r="O4" s="33"/>
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
-      <c r="R4" s="41" t="s">
+      <c r="R4" s="35" t="s">
         <v>97</v>
       </c>
       <c r="S4" s="18"/>
@@ -3532,7 +3567,7 @@
       <c r="V4" s="18"/>
       <c r="W4" s="18"/>
       <c r="X4" s="18"/>
-      <c r="Y4" s="43" t="s">
+      <c r="Y4" s="37" t="s">
         <v>101</v>
       </c>
       <c r="Z4" s="18"/>
@@ -3541,7 +3576,7 @@
       <c r="AC4" s="18"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="25">
+      <c r="A5" s="23">
         <v>2.2000000000000002</v>
       </c>
       <c r="B5" s="18"/>
@@ -3551,7 +3586,7 @@
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
-      <c r="I5" s="26">
+      <c r="I5" s="24">
         <v>2.2000000000000002</v>
       </c>
       <c r="J5" s="18"/>
@@ -3559,12 +3594,12 @@
       <c r="L5" s="18"/>
       <c r="M5" s="18"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="38" t="s">
+      <c r="O5" s="32" t="s">
         <v>90</v>
       </c>
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
-      <c r="R5" s="41" t="s">
+      <c r="R5" s="35" t="s">
         <v>98</v>
       </c>
       <c r="S5" s="18"/>
@@ -3573,7 +3608,7 @@
       <c r="V5" s="18"/>
       <c r="W5" s="18"/>
       <c r="X5" s="18"/>
-      <c r="Y5" s="43" t="s">
+      <c r="Y5" s="37" t="s">
         <v>102</v>
       </c>
       <c r="Z5" s="18"/>
@@ -3582,7 +3617,7 @@
       <c r="AC5" s="18"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="33">
+      <c r="A6" s="31">
         <v>2.2999999999999998</v>
       </c>
       <c r="B6" s="18"/>
@@ -3593,19 +3628,19 @@
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
-      <c r="J6" s="26">
+      <c r="J6" s="24">
         <v>2.2999999999999998</v>
       </c>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
-      <c r="O6" s="38" t="s">
+      <c r="O6" s="32" t="s">
         <v>91</v>
       </c>
       <c r="P6" s="18"/>
       <c r="Q6" s="18"/>
-      <c r="R6" s="41" t="s">
+      <c r="R6" s="35" t="s">
         <v>99</v>
       </c>
       <c r="S6" s="18"/>
@@ -3614,7 +3649,7 @@
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
       <c r="X6" s="18"/>
-      <c r="Y6" s="43" t="s">
+      <c r="Y6" s="37" t="s">
         <v>94</v>
       </c>
       <c r="Z6" s="18"/>
@@ -3635,31 +3670,31 @@
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
-      <c r="K7" s="23" t="s">
+      <c r="K7" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="38" t="s">
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="P7" s="23" t="s">
+      <c r="P7" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="41" t="s">
+      <c r="Q7" s="43"/>
+      <c r="R7" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="S7" s="23" t="s">
+      <c r="S7" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="T7" s="24"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="24"/>
+      <c r="T7" s="43"/>
+      <c r="U7" s="43"/>
+      <c r="V7" s="43"/>
       <c r="W7" s="18"/>
       <c r="X7" s="18"/>
-      <c r="Y7" s="43" t="s">
+      <c r="Y7" s="37" t="s">
         <v>98</v>
       </c>
       <c r="Z7" s="18"/>
@@ -3668,7 +3703,7 @@
       <c r="AC7" s="18"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="A8" s="23">
         <v>3.1</v>
       </c>
       <c r="B8" s="18"/>
@@ -3680,18 +3715,18 @@
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
-      <c r="K8" s="34">
+      <c r="K8" s="40">
         <v>3.1</v>
       </c>
-      <c r="L8" s="35"/>
+      <c r="L8" s="41"/>
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
-      <c r="O8" s="38" t="s">
+      <c r="O8" s="32" t="s">
         <v>92</v>
       </c>
       <c r="P8" s="18"/>
       <c r="Q8" s="18"/>
-      <c r="R8" s="41" t="s">
+      <c r="R8" s="35" t="s">
         <v>95</v>
       </c>
       <c r="S8" s="18"/>
@@ -3700,7 +3735,7 @@
       <c r="V8" s="18"/>
       <c r="W8" s="18"/>
       <c r="X8" s="18"/>
-      <c r="Y8" s="43" t="s">
+      <c r="Y8" s="37" t="s">
         <v>99</v>
       </c>
       <c r="Z8" s="18"/>
@@ -3709,7 +3744,7 @@
       <c r="AC8" s="18"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="25">
+      <c r="A9" s="23">
         <v>3.2</v>
       </c>
       <c r="B9" s="18"/>
@@ -3723,14 +3758,14 @@
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
-      <c r="M9" s="34">
+      <c r="M9" s="40">
         <v>3.2</v>
       </c>
-      <c r="N9" s="35"/>
-      <c r="O9" s="38"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="32"/>
       <c r="P9" s="18"/>
       <c r="Q9" s="18"/>
-      <c r="R9" s="41" t="s">
+      <c r="R9" s="35" t="s">
         <v>94</v>
       </c>
       <c r="S9" s="18"/>
@@ -3739,7 +3774,7 @@
       <c r="V9" s="18"/>
       <c r="W9" s="18"/>
       <c r="X9" s="18"/>
-      <c r="Y9" s="43" t="s">
+      <c r="Y9" s="37" t="s">
         <v>103</v>
       </c>
       <c r="Z9" s="18"/>
@@ -3748,7 +3783,7 @@
       <c r="AC9" s="18"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="25">
+      <c r="A10" s="23">
         <v>3.3</v>
       </c>
       <c r="B10" s="18"/>
@@ -3764,28 +3799,28 @@
       <c r="L10" s="18"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="38" t="s">
+      <c r="O10" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="P10" s="34">
+      <c r="P10" s="40">
         <v>3.3</v>
       </c>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="35"/>
       <c r="S10" s="18"/>
       <c r="T10" s="18"/>
       <c r="U10" s="18"/>
       <c r="V10" s="18"/>
       <c r="W10" s="18"/>
       <c r="X10" s="18"/>
-      <c r="Y10" s="43"/>
+      <c r="Y10" s="37"/>
       <c r="Z10" s="18"/>
       <c r="AA10" s="18"/>
       <c r="AB10" s="18"/>
       <c r="AC10" s="18"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="25">
+      <c r="A11" s="23">
         <v>3.4</v>
       </c>
       <c r="B11" s="18"/>
@@ -3801,23 +3836,23 @@
       <c r="L11" s="18"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="38" t="s">
+      <c r="O11" s="32" t="s">
         <v>94</v>
       </c>
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
-      <c r="R11" s="41" t="s">
+      <c r="R11" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="S11" s="34">
+      <c r="S11" s="40">
         <v>3.4</v>
       </c>
-      <c r="T11" s="35"/>
+      <c r="T11" s="41"/>
       <c r="U11" s="18"/>
       <c r="V11" s="18"/>
       <c r="W11" s="18"/>
       <c r="X11" s="18"/>
-      <c r="Y11" s="43" t="s">
+      <c r="Y11" s="37" t="s">
         <v>93</v>
       </c>
       <c r="Z11" s="18"/>
@@ -3826,7 +3861,7 @@
       <c r="AC11" s="18"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="25">
+      <c r="A12" s="23">
         <v>3.5</v>
       </c>
       <c r="B12" s="18"/>
@@ -3842,23 +3877,23 @@
       <c r="L12" s="18"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
-      <c r="O12" s="38" t="s">
+      <c r="O12" s="32" t="s">
         <v>95</v>
       </c>
       <c r="P12" s="18"/>
       <c r="Q12" s="18"/>
-      <c r="R12" s="41" t="s">
+      <c r="R12" s="35" t="s">
         <v>94</v>
       </c>
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
-      <c r="U12" s="36">
+      <c r="U12" s="44">
         <v>3.5</v>
       </c>
-      <c r="V12" s="37"/>
+      <c r="V12" s="45"/>
       <c r="W12" s="18"/>
       <c r="X12" s="18"/>
-      <c r="Y12" s="43" t="s">
+      <c r="Y12" s="37" t="s">
         <v>94</v>
       </c>
       <c r="Z12" s="18"/>
@@ -3883,34 +3918,34 @@
       <c r="L13" s="18"/>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
-      <c r="O13" s="38" t="s">
+      <c r="O13" s="32" t="s">
         <v>91</v>
       </c>
       <c r="P13" s="18"/>
       <c r="Q13" s="18"/>
-      <c r="R13" s="41" t="s">
+      <c r="R13" s="35" t="s">
         <v>95</v>
       </c>
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
       <c r="U13" s="18"/>
       <c r="V13" s="18"/>
-      <c r="W13" s="23" t="s">
+      <c r="W13" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="X13" s="24"/>
-      <c r="Y13" s="43" t="s">
+      <c r="X13" s="43"/>
+      <c r="Y13" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="Z13" s="23" t="s">
+      <c r="Z13" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="23"/>
-      <c r="AC13" s="23"/>
+      <c r="AA13" s="42"/>
+      <c r="AB13" s="42"/>
+      <c r="AC13" s="42"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="25">
+      <c r="A14" s="23">
         <v>4.0999999999999996</v>
       </c>
       <c r="B14" s="18"/>
@@ -3926,23 +3961,23 @@
       <c r="L14" s="18"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="38" t="s">
+      <c r="O14" s="32" t="s">
         <v>96</v>
       </c>
       <c r="P14" s="18"/>
       <c r="Q14" s="18"/>
-      <c r="R14" s="41" t="s">
+      <c r="R14" s="35" t="s">
         <v>91</v>
       </c>
       <c r="S14" s="18"/>
       <c r="T14" s="18"/>
       <c r="U14" s="18"/>
       <c r="V14" s="18"/>
-      <c r="W14" s="26">
+      <c r="W14" s="24">
         <v>4.0999999999999996</v>
       </c>
       <c r="X14" s="1"/>
-      <c r="Y14" s="43" t="s">
+      <c r="Y14" s="37" t="s">
         <v>91</v>
       </c>
       <c r="Z14" s="18"/>
@@ -3951,7 +3986,7 @@
       <c r="AC14" s="18"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="25">
+      <c r="A15" s="23">
         <v>4.2</v>
       </c>
       <c r="B15" s="18"/>
@@ -3967,10 +4002,10 @@
       <c r="L15" s="18"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="38"/>
+      <c r="O15" s="32"/>
       <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
-      <c r="R15" s="41" t="s">
+      <c r="R15" s="35" t="s">
         <v>96</v>
       </c>
       <c r="S15" s="18"/>
@@ -3978,10 +4013,10 @@
       <c r="U15" s="18"/>
       <c r="V15" s="18"/>
       <c r="W15" s="18"/>
-      <c r="X15" s="42">
+      <c r="X15" s="36">
         <v>4.2</v>
       </c>
-      <c r="Y15" s="43" t="s">
+      <c r="Y15" s="37" t="s">
         <v>96</v>
       </c>
       <c r="Z15" s="18"/>
@@ -3990,7 +4025,7 @@
       <c r="AC15" s="18"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="25">
+      <c r="A16" s="23">
         <v>4.3</v>
       </c>
       <c r="B16" s="18"/>
@@ -4006,18 +4041,18 @@
       <c r="L16" s="18"/>
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="38"/>
+      <c r="O16" s="32"/>
       <c r="P16" s="18"/>
       <c r="Q16" s="18"/>
-      <c r="R16" s="41"/>
+      <c r="R16" s="35"/>
       <c r="S16" s="18"/>
       <c r="T16" s="18"/>
       <c r="U16" s="18"/>
       <c r="V16" s="18"/>
       <c r="W16" s="18"/>
       <c r="X16" s="18"/>
-      <c r="Y16" s="43"/>
-      <c r="Z16" s="29">
+      <c r="Y16" s="37"/>
+      <c r="Z16" s="27">
         <v>4.2</v>
       </c>
       <c r="AA16" s="18"/>
@@ -4025,7 +4060,7 @@
       <c r="AC16" s="18"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="25">
+      <c r="A17" s="23">
         <v>4.4000000000000004</v>
       </c>
       <c r="B17" s="18"/>
@@ -4041,26 +4076,26 @@
       <c r="L17" s="18"/>
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
-      <c r="O17" s="38"/>
+      <c r="O17" s="32"/>
       <c r="P17" s="18"/>
       <c r="Q17" s="18"/>
-      <c r="R17" s="41"/>
+      <c r="R17" s="35"/>
       <c r="S17" s="18"/>
       <c r="T17" s="18"/>
       <c r="U17" s="18"/>
       <c r="V17" s="18"/>
       <c r="W17" s="18"/>
       <c r="X17" s="18"/>
-      <c r="Y17" s="43"/>
+      <c r="Y17" s="37"/>
       <c r="Z17" s="18"/>
-      <c r="AA17" s="26">
+      <c r="AA17" s="24">
         <v>4.4000000000000004</v>
       </c>
       <c r="AB17" s="18"/>
       <c r="AC17" s="18"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="25">
+      <c r="A18" s="23">
         <v>4.5</v>
       </c>
       <c r="B18" s="18"/>
@@ -4076,23 +4111,23 @@
       <c r="L18" s="18"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
-      <c r="O18" s="38"/>
+      <c r="O18" s="32"/>
       <c r="P18" s="18"/>
       <c r="Q18" s="18"/>
-      <c r="R18" s="41"/>
+      <c r="R18" s="35"/>
       <c r="S18" s="18"/>
       <c r="T18" s="18"/>
       <c r="U18" s="18"/>
       <c r="V18" s="18"/>
       <c r="W18" s="18"/>
       <c r="X18" s="18"/>
-      <c r="Y18" s="43"/>
+      <c r="Y18" s="37"/>
       <c r="Z18" s="18"/>
       <c r="AA18" s="18"/>
-      <c r="AB18" s="34">
+      <c r="AB18" s="40">
         <v>4.5</v>
       </c>
-      <c r="AC18" s="35"/>
+      <c r="AC18" s="41"/>
     </row>
     <row r="19" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
@@ -4112,6 +4147,12 @@
     <row r="34" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="35" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="36" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="37" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="38" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="39" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="40" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="41" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="42" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="AB18:AC18"/>
@@ -4137,7 +4178,7 @@
   <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4145,8 +4186,8 @@
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" style="11" customWidth="1"/>
     <col min="3" max="3" width="5" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="24" width="5.85546875" style="11" customWidth="1"/>
-    <col min="25" max="25" width="9.42578125" customWidth="1"/>
+    <col min="4" max="23" width="5.85546875" style="11" customWidth="1"/>
+    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -4254,9 +4295,19 @@
       <c r="J2" s="14">
         <v>8</v>
       </c>
+      <c r="L2" s="11">
+        <v>7</v>
+      </c>
+      <c r="M2" s="11">
+        <v>8</v>
+      </c>
+      <c r="N2" s="11">
+        <v>8</v>
+      </c>
+      <c r="X2" s="16"/>
       <c r="Y2">
-        <f>AVERAGE(B2:X2)</f>
-        <v>6.4444444444444446</v>
+        <f>AVERAGE(B2:W2)</f>
+        <v>6.75</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -4290,9 +4341,19 @@
       <c r="J3" s="14">
         <v>8</v>
       </c>
+      <c r="L3" s="11">
+        <v>6</v>
+      </c>
+      <c r="M3" s="11">
+        <v>7</v>
+      </c>
+      <c r="N3" s="11">
+        <v>7</v>
+      </c>
+      <c r="X3" s="16"/>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y7" si="0">AVERAGE(B3:X3)</f>
-        <v>6.333333333333333</v>
+        <f>AVERAGE(B3:W3)</f>
+        <v>6.416666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -4326,9 +4387,19 @@
       <c r="J4" s="14">
         <v>7</v>
       </c>
+      <c r="L4" s="11">
+        <v>6</v>
+      </c>
+      <c r="M4" s="11">
+        <v>6</v>
+      </c>
+      <c r="N4" s="11">
+        <v>6</v>
+      </c>
+      <c r="X4" s="16"/>
       <c r="Y4">
-        <f t="shared" si="0"/>
-        <v>6.333333333333333</v>
+        <f>AVERAGE(B4:W4)</f>
+        <v>6.25</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -4362,9 +4433,19 @@
       <c r="J5" s="14">
         <v>8</v>
       </c>
+      <c r="L5" s="11">
+        <v>7</v>
+      </c>
+      <c r="M5" s="11">
+        <v>6</v>
+      </c>
+      <c r="N5" s="11">
+        <v>7</v>
+      </c>
+      <c r="X5" s="16"/>
       <c r="Y5">
-        <f t="shared" si="0"/>
-        <v>6.333333333333333</v>
+        <f>AVERAGE(B5:W5)</f>
+        <v>6.416666666666667</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4398,9 +4479,19 @@
       <c r="J6" s="14">
         <v>9</v>
       </c>
+      <c r="L6" s="11">
+        <v>7</v>
+      </c>
+      <c r="M6" s="11">
+        <v>8</v>
+      </c>
+      <c r="N6" s="11">
+        <v>9</v>
+      </c>
+      <c r="X6" s="16"/>
       <c r="Y6">
-        <f t="shared" si="0"/>
-        <v>6.5555555555555554</v>
+        <f>AVERAGE(B6:W6)</f>
+        <v>6.916666666666667</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4408,44 +4499,100 @@
         <v>81</v>
       </c>
       <c r="B7" s="14">
-        <f t="shared" ref="B7:J7" si="1">SUM(B2:B6)</f>
+        <f t="shared" ref="B7:X7" si="0">SUM(B2:B6)</f>
         <v>11</v>
       </c>
       <c r="C7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="D7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="E7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="F7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="G7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="H7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="I7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="J7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
+      <c r="K7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="16">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="M7" s="16">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="N7" s="16">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="O7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="Y7">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <f>AVERAGE(B7:W7)</f>
+        <v>17.863636363636363</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -4461,88 +4608,88 @@
         <v>52</v>
       </c>
       <c r="D8" s="12">
-        <f t="shared" ref="D8:X8" si="2">C8+D7</f>
+        <f t="shared" ref="D8:X8" si="1">C8+D7</f>
         <v>93</v>
       </c>
       <c r="E8" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="F8" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>154</v>
       </c>
       <c r="G8" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>187</v>
       </c>
       <c r="H8" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>220</v>
       </c>
       <c r="I8" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>248</v>
       </c>
       <c r="J8" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>288</v>
       </c>
       <c r="K8" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>288</v>
       </c>
       <c r="L8" s="12">
-        <f t="shared" si="2"/>
-        <v>288</v>
+        <f t="shared" si="1"/>
+        <v>321</v>
       </c>
       <c r="M8" s="12">
-        <f t="shared" si="2"/>
-        <v>288</v>
+        <f t="shared" si="1"/>
+        <v>356</v>
       </c>
       <c r="N8" s="12">
-        <f t="shared" si="2"/>
-        <v>288</v>
+        <f t="shared" si="1"/>
+        <v>393</v>
       </c>
       <c r="O8" s="12">
-        <f t="shared" si="2"/>
-        <v>288</v>
+        <f t="shared" si="1"/>
+        <v>393</v>
       </c>
       <c r="P8" s="12">
-        <f t="shared" si="2"/>
-        <v>288</v>
+        <f t="shared" si="1"/>
+        <v>393</v>
       </c>
       <c r="Q8" s="12">
-        <f t="shared" si="2"/>
-        <v>288</v>
+        <f t="shared" si="1"/>
+        <v>393</v>
       </c>
       <c r="R8" s="12">
-        <f t="shared" si="2"/>
-        <v>288</v>
+        <f t="shared" si="1"/>
+        <v>393</v>
       </c>
       <c r="S8" s="12">
-        <f t="shared" si="2"/>
-        <v>288</v>
+        <f t="shared" si="1"/>
+        <v>393</v>
       </c>
       <c r="T8" s="12">
-        <f t="shared" si="2"/>
-        <v>288</v>
+        <f t="shared" si="1"/>
+        <v>393</v>
       </c>
       <c r="U8" s="12">
-        <f t="shared" si="2"/>
-        <v>288</v>
+        <f t="shared" si="1"/>
+        <v>393</v>
       </c>
       <c r="V8" s="12">
-        <f t="shared" si="2"/>
-        <v>288</v>
+        <f t="shared" si="1"/>
+        <v>393</v>
       </c>
       <c r="W8" s="12">
-        <f t="shared" si="2"/>
-        <v>288</v>
-      </c>
-      <c r="X8" s="12">
-        <f t="shared" si="2"/>
-        <v>288</v>
+        <f t="shared" si="1"/>
+        <v>393</v>
+      </c>
+      <c r="X8" s="16">
+        <f t="shared" si="1"/>
+        <v>393</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -4559,7 +4706,6 @@
       <c r="U13"/>
       <c r="V13"/>
       <c r="W13"/>
-      <c r="X13"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
@@ -4575,7 +4721,6 @@
       <c r="U14"/>
       <c r="V14"/>
       <c r="W14"/>
-      <c r="X14"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
@@ -4591,7 +4736,6 @@
       <c r="U15"/>
       <c r="V15"/>
       <c r="W15"/>
-      <c r="X15"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
@@ -4607,9 +4751,8 @@
       <c r="U16"/>
       <c r="V16"/>
       <c r="W16"/>
-      <c r="X16"/>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="L17"/>
       <c r="M17"/>
@@ -4623,9 +4766,8 @@
       <c r="U17"/>
       <c r="V17"/>
       <c r="W17"/>
-      <c r="X17"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="L18"/>
       <c r="M18"/>
@@ -4639,9 +4781,8 @@
       <c r="U18"/>
       <c r="V18"/>
       <c r="W18"/>
-      <c r="X18"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="L19"/>
       <c r="M19"/>
@@ -4655,9 +4796,8 @@
       <c r="U19"/>
       <c r="V19"/>
       <c r="W19"/>
-      <c r="X19"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="L20"/>
       <c r="M20"/>
@@ -4671,9 +4811,8 @@
       <c r="U20"/>
       <c r="V20"/>
       <c r="W20"/>
-      <c r="X20"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="L21"/>
       <c r="M21"/>
@@ -4687,7 +4826,6 @@
       <c r="U21"/>
       <c r="V21"/>
       <c r="W21"/>
-      <c r="X21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed Weekly Reports & Updated WBS
</commit_message>
<xml_diff>
--- a/Content/WBS.xlsx
+++ b/Content/WBS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BluSh3ll\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6F7C5C-A475-4C23-B705-2D2674A9F193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAD51A1-503B-4E82-86F3-31979F3BF781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
   <si>
     <t>ID</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>WB</t>
   </si>
 </sst>
 </file>
@@ -383,7 +386,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,6 +432,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -521,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -628,6 +643,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -644,6 +662,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -751,9 +787,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Team Hours'!$B$1:$W$1</c:f>
+              <c:f>'Team Hours'!$B$1:$X$1</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>Wk5</c:v>
                 </c:pt>
@@ -791,33 +827,36 @@
                   <c:v>Wk16</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>WB</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>Wk17</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Wk18</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Wk19</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Wk20</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Wk21</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>Wk22</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Wk23</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Wk24</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>Wk25</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>Wk26</c:v>
                 </c:pt>
               </c:strCache>
@@ -825,10 +864,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Team Hours'!$B$7:$W$7</c:f>
+              <c:f>'Team Hours'!$B$7:$X$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>11</c:v>
                 </c:pt>
@@ -856,44 +895,35 @@
                 <c:pt idx="8">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="10">
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>37</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1154,9 +1184,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Team Hours'!$B$1:$W$1</c:f>
+              <c:f>'Team Hours'!$B$1:$X$1</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>Wk5</c:v>
                 </c:pt>
@@ -1194,33 +1224,36 @@
                   <c:v>Wk16</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>WB</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>Wk17</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Wk18</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Wk19</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Wk20</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Wk21</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>Wk22</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Wk23</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Wk24</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>Wk25</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>Wk26</c:v>
                 </c:pt>
               </c:strCache>
@@ -1228,10 +1261,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Team Hours'!$B$8:$W$8</c:f>
+              <c:f>'Team Hours'!$B$8:$X$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>11</c:v>
                 </c:pt>
@@ -1259,44 +1292,35 @@
                 <c:pt idx="8">
                   <c:v>288</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>288</c:v>
-                </c:pt>
                 <c:pt idx="10">
                   <c:v>321</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>356</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>393</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>393</c:v>
+                  <c:v>389</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>393</c:v>
+                  <c:v>424</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>393</c:v>
+                  <c:v>462</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>393</c:v>
+                  <c:v>501</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>393</c:v>
+                  <c:v>537</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>393</c:v>
+                  <c:v>596</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>393</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>393</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>393</c:v>
+                  <c:v>653</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2639,7 +2663,7 @@
       <xdr:rowOff>34739</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>67235</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>145678</xdr:rowOff>
@@ -2936,7 +2960,7 @@
   <dimension ref="A1:AI18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="G11" sqref="A11:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3185,7 +3209,7 @@
       <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="40" t="s">
         <v>77</v>
       </c>
       <c r="E11" s="9">
@@ -3208,7 +3232,7 @@
       <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="10">
         <v>43499</v>
       </c>
@@ -3229,7 +3253,7 @@
       <c r="C13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="39"/>
+      <c r="D13" s="40"/>
       <c r="E13" s="8">
         <v>43513</v>
       </c>
@@ -3250,7 +3274,7 @@
       <c r="C14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="39"/>
+      <c r="D14" s="40"/>
       <c r="E14" s="10">
         <v>43513</v>
       </c>
@@ -3271,7 +3295,7 @@
       <c r="C15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="39"/>
+      <c r="D15" s="40"/>
       <c r="E15" s="10">
         <v>43520</v>
       </c>
@@ -3292,7 +3316,7 @@
       <c r="C16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="39"/>
+      <c r="D16" s="40"/>
       <c r="E16" s="9">
         <v>43526</v>
       </c>
@@ -3313,7 +3337,7 @@
       <c r="C17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="39"/>
+      <c r="D17" s="40"/>
       <c r="E17" s="9">
         <v>43540</v>
       </c>
@@ -3334,7 +3358,7 @@
       <c r="C18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="39"/>
+      <c r="D18" s="40"/>
       <c r="E18" s="10">
         <v>43547</v>
       </c>
@@ -3359,8 +3383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF51B197-A615-4074-96E4-CE4CCB37617D}">
   <dimension ref="A1:AC42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3470,14 +3494,14 @@
       <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
@@ -3511,11 +3535,11 @@
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
@@ -3670,28 +3694,28 @@
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
-      <c r="K7" s="42" t="s">
+      <c r="K7" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
       <c r="O7" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="P7" s="42" t="s">
+      <c r="P7" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="43"/>
+      <c r="Q7" s="44"/>
       <c r="R7" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="S7" s="42" t="s">
+      <c r="S7" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="T7" s="43"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="43"/>
+      <c r="T7" s="44"/>
+      <c r="U7" s="44"/>
+      <c r="V7" s="44"/>
       <c r="W7" s="18"/>
       <c r="X7" s="18"/>
       <c r="Y7" s="37" t="s">
@@ -3715,10 +3739,10 @@
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
-      <c r="K8" s="40">
+      <c r="K8" s="41">
         <v>3.1</v>
       </c>
-      <c r="L8" s="41"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
       <c r="O8" s="32" t="s">
@@ -3758,10 +3782,10 @@
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
-      <c r="M9" s="40">
+      <c r="M9" s="41">
         <v>3.2</v>
       </c>
-      <c r="N9" s="41"/>
+      <c r="N9" s="42"/>
       <c r="O9" s="32"/>
       <c r="P9" s="18"/>
       <c r="Q9" s="18"/>
@@ -3802,10 +3826,10 @@
       <c r="O10" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="P10" s="40">
+      <c r="P10" s="41">
         <v>3.3</v>
       </c>
-      <c r="Q10" s="41"/>
+      <c r="Q10" s="42"/>
       <c r="R10" s="35"/>
       <c r="S10" s="18"/>
       <c r="T10" s="18"/>
@@ -3844,10 +3868,10 @@
       <c r="R11" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="S11" s="40">
+      <c r="S11" s="41">
         <v>3.4</v>
       </c>
-      <c r="T11" s="41"/>
+      <c r="T11" s="42"/>
       <c r="U11" s="18"/>
       <c r="V11" s="18"/>
       <c r="W11" s="18"/>
@@ -3887,10 +3911,10 @@
       </c>
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
-      <c r="U12" s="44">
+      <c r="U12" s="45">
         <v>3.5</v>
       </c>
-      <c r="V12" s="45"/>
+      <c r="V12" s="46"/>
       <c r="W12" s="18"/>
       <c r="X12" s="18"/>
       <c r="Y12" s="37" t="s">
@@ -3930,19 +3954,19 @@
       <c r="T13" s="18"/>
       <c r="U13" s="18"/>
       <c r="V13" s="18"/>
-      <c r="W13" s="42" t="s">
+      <c r="W13" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="X13" s="43"/>
+      <c r="X13" s="44"/>
       <c r="Y13" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="Z13" s="42" t="s">
+      <c r="Z13" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="AA13" s="42"/>
-      <c r="AB13" s="42"/>
-      <c r="AC13" s="42"/>
+      <c r="AA13" s="43"/>
+      <c r="AB13" s="43"/>
+      <c r="AC13" s="43"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="23">
@@ -4124,10 +4148,10 @@
       <c r="Y18" s="37"/>
       <c r="Z18" s="18"/>
       <c r="AA18" s="18"/>
-      <c r="AB18" s="40">
+      <c r="AB18" s="41">
         <v>4.5</v>
       </c>
-      <c r="AC18" s="41"/>
+      <c r="AC18" s="42"/>
     </row>
     <row r="19" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
@@ -4175,10 +4199,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C261B442-2F63-4F7C-A433-D2B145AB0897}">
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4186,11 +4210,13 @@
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" style="11" customWidth="1"/>
     <col min="3" max="3" width="5" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="23" width="5.85546875" style="11" customWidth="1"/>
-    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="5.85546875" style="11" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" style="39" customWidth="1"/>
+    <col min="15" max="24" width="5.85546875" style="11" customWidth="1"/>
+    <col min="25" max="25" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>46</v>
       </c>
@@ -4218,7 +4244,7 @@
       <c r="J1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="49" t="s">
         <v>55</v>
       </c>
       <c r="L1" s="4" t="s">
@@ -4227,44 +4253,47 @@
       <c r="M1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="U1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -4295,22 +4324,47 @@
       <c r="J2" s="14">
         <v>8</v>
       </c>
+      <c r="K2" s="50"/>
       <c r="L2" s="11">
         <v>7</v>
       </c>
       <c r="M2" s="11">
         <v>8</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="48"/>
+      <c r="O2" s="11">
+        <v>7</v>
+      </c>
+      <c r="P2" s="11">
         <v>8</v>
       </c>
-      <c r="X2" s="16"/>
-      <c r="Y2">
-        <f>AVERAGE(B2:W2)</f>
-        <v>6.75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q2" s="11">
+        <v>8</v>
+      </c>
+      <c r="R2" s="11">
+        <v>10</v>
+      </c>
+      <c r="S2" s="11">
+        <v>7</v>
+      </c>
+      <c r="T2" s="11">
+        <v>13</v>
+      </c>
+      <c r="U2" s="11">
+        <v>14</v>
+      </c>
+      <c r="V2" s="52"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="11">
+        <v>15</v>
+      </c>
+      <c r="Y2" s="16"/>
+      <c r="Z2">
+        <f t="shared" ref="Z2:Z7" si="0">AVERAGE(B2:X2)</f>
+        <v>8.1578947368421044</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -4341,22 +4395,47 @@
       <c r="J3" s="14">
         <v>8</v>
       </c>
+      <c r="K3" s="50"/>
       <c r="L3" s="11">
         <v>6</v>
       </c>
       <c r="M3" s="11">
         <v>7</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="48"/>
+      <c r="O3" s="11">
+        <v>6</v>
+      </c>
+      <c r="P3" s="11">
         <v>7</v>
       </c>
-      <c r="X3" s="16"/>
-      <c r="Y3">
-        <f>AVERAGE(B3:W3)</f>
-        <v>6.416666666666667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q3" s="11">
+        <v>7</v>
+      </c>
+      <c r="R3" s="11">
+        <v>6</v>
+      </c>
+      <c r="S3" s="11">
+        <v>6</v>
+      </c>
+      <c r="T3" s="11">
+        <v>7</v>
+      </c>
+      <c r="U3" s="11">
+        <v>11</v>
+      </c>
+      <c r="V3" s="52"/>
+      <c r="W3" s="52"/>
+      <c r="X3" s="11">
+        <v>14</v>
+      </c>
+      <c r="Y3" s="16"/>
+      <c r="Z3">
+        <f t="shared" si="0"/>
+        <v>7.0526315789473681</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -4387,22 +4466,47 @@
       <c r="J4" s="14">
         <v>7</v>
       </c>
+      <c r="K4" s="50"/>
       <c r="L4" s="11">
         <v>6</v>
       </c>
       <c r="M4" s="11">
         <v>6</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="48"/>
+      <c r="O4" s="11">
         <v>6</v>
       </c>
-      <c r="X4" s="16"/>
-      <c r="Y4">
-        <f>AVERAGE(B4:W4)</f>
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P4" s="11">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>7</v>
+      </c>
+      <c r="R4" s="11">
+        <v>6</v>
+      </c>
+      <c r="S4" s="11">
+        <v>6</v>
+      </c>
+      <c r="T4" s="11">
+        <v>13</v>
+      </c>
+      <c r="U4" s="11">
+        <v>9</v>
+      </c>
+      <c r="V4" s="52"/>
+      <c r="W4" s="52"/>
+      <c r="X4" s="11">
+        <v>14</v>
+      </c>
+      <c r="Y4" s="16"/>
+      <c r="Z4">
+        <f t="shared" si="0"/>
+        <v>7.1578947368421053</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -4433,22 +4537,47 @@
       <c r="J5" s="14">
         <v>8</v>
       </c>
+      <c r="K5" s="50"/>
       <c r="L5" s="11">
         <v>7</v>
       </c>
       <c r="M5" s="11">
         <v>6</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="48"/>
+      <c r="O5" s="11">
         <v>7</v>
       </c>
-      <c r="X5" s="16"/>
-      <c r="Y5">
-        <f>AVERAGE(B5:W5)</f>
-        <v>6.416666666666667</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="11">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>7</v>
+      </c>
+      <c r="R5" s="11">
+        <v>5</v>
+      </c>
+      <c r="S5" s="11">
+        <v>5</v>
+      </c>
+      <c r="T5" s="11">
+        <v>12</v>
+      </c>
+      <c r="U5" s="11">
+        <v>11</v>
+      </c>
+      <c r="V5" s="52"/>
+      <c r="W5" s="52"/>
+      <c r="X5" s="11">
+        <v>12</v>
+      </c>
+      <c r="Y5" s="16"/>
+      <c r="Z5">
+        <f t="shared" si="0"/>
+        <v>7.1052631578947372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -4479,123 +4608,140 @@
       <c r="J6" s="14">
         <v>9</v>
       </c>
+      <c r="K6" s="50"/>
       <c r="L6" s="11">
         <v>7</v>
       </c>
       <c r="M6" s="11">
         <v>8</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="48"/>
+      <c r="O6" s="11">
+        <v>7</v>
+      </c>
+      <c r="P6" s="11">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="11">
         <v>9</v>
       </c>
-      <c r="X6" s="16"/>
-      <c r="Y6">
-        <f>AVERAGE(B6:W6)</f>
-        <v>6.916666666666667</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R6" s="11">
+        <v>12</v>
+      </c>
+      <c r="S6" s="11">
+        <v>12</v>
+      </c>
+      <c r="T6" s="11">
+        <v>14</v>
+      </c>
+      <c r="U6" s="11">
+        <v>12</v>
+      </c>
+      <c r="V6" s="52"/>
+      <c r="W6" s="52"/>
+      <c r="X6" s="11">
+        <v>16</v>
+      </c>
+      <c r="Y6" s="16"/>
+      <c r="Z6">
+        <f t="shared" si="0"/>
+        <v>8.6315789473684212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>81</v>
       </c>
       <c r="B7" s="14">
-        <f t="shared" ref="B7:X7" si="0">SUM(B2:B6)</f>
+        <f t="shared" ref="B7:Y7" si="1">SUM(B2:B6)</f>
         <v>11</v>
       </c>
       <c r="C7" s="14">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="D7" s="14">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="K7" s="50"/>
+      <c r="L7" s="16">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="M7" s="16">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="N7" s="48"/>
+      <c r="O7" s="16">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="P7" s="16">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="Q7" s="16">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="R7" s="16">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="S7" s="16">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="T7" s="16">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="U7" s="39">
+        <f t="shared" ref="U7" si="2">SUM(U2:U6)</f>
+        <v>57</v>
+      </c>
+      <c r="V7" s="52"/>
+      <c r="W7" s="52"/>
+      <c r="X7" s="16">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="Y7" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z7">
         <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="D7" s="14">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="E7" s="14">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="F7" s="14">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G7" s="14">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="H7" s="14">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="I7" s="14">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="J7" s="14">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="K7" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="16">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="M7" s="16">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="N7" s="16">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="O7" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S7" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T7" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U7" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V7" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W7" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="X7" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <f>AVERAGE(B7:W7)</f>
-        <v>17.863636363636363</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+        <v>38.10526315789474</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -4608,91 +4754,83 @@
         <v>52</v>
       </c>
       <c r="D8" s="12">
-        <f t="shared" ref="D8:X8" si="1">C8+D7</f>
+        <f t="shared" ref="D8:Y8" si="3">C8+D7</f>
         <v>93</v>
       </c>
       <c r="E8" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="F8" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>154</v>
       </c>
       <c r="G8" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>187</v>
       </c>
       <c r="H8" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>220</v>
       </c>
       <c r="I8" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>248</v>
       </c>
       <c r="J8" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>288</v>
       </c>
-      <c r="K8" s="12">
-        <f t="shared" si="1"/>
-        <v>288</v>
-      </c>
+      <c r="K8" s="50"/>
       <c r="L8" s="12">
-        <f t="shared" si="1"/>
+        <f>J8+L7</f>
         <v>321</v>
       </c>
       <c r="M8" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>356</v>
       </c>
-      <c r="N8" s="12">
-        <f t="shared" si="1"/>
-        <v>393</v>
-      </c>
+      <c r="N8" s="48"/>
       <c r="O8" s="12">
-        <f t="shared" si="1"/>
-        <v>393</v>
+        <f>M8+O7</f>
+        <v>389</v>
       </c>
       <c r="P8" s="12">
-        <f t="shared" si="1"/>
-        <v>393</v>
+        <f t="shared" si="3"/>
+        <v>424</v>
       </c>
       <c r="Q8" s="12">
-        <f t="shared" si="1"/>
-        <v>393</v>
+        <f t="shared" si="3"/>
+        <v>462</v>
       </c>
       <c r="R8" s="12">
-        <f t="shared" si="1"/>
-        <v>393</v>
+        <f t="shared" si="3"/>
+        <v>501</v>
       </c>
       <c r="S8" s="12">
-        <f t="shared" si="1"/>
-        <v>393</v>
+        <f t="shared" si="3"/>
+        <v>537</v>
       </c>
       <c r="T8" s="12">
-        <f t="shared" si="1"/>
-        <v>393</v>
-      </c>
-      <c r="U8" s="12">
-        <f t="shared" si="1"/>
-        <v>393</v>
-      </c>
-      <c r="V8" s="12">
-        <f t="shared" si="1"/>
-        <v>393</v>
-      </c>
-      <c r="W8" s="12">
-        <f t="shared" si="1"/>
-        <v>393</v>
-      </c>
-      <c r="X8" s="16">
-        <f t="shared" si="1"/>
-        <v>393</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>596</v>
+      </c>
+      <c r="U8" s="39">
+        <f t="shared" si="3"/>
+        <v>653</v>
+      </c>
+      <c r="V8" s="52"/>
+      <c r="W8" s="52"/>
+      <c r="X8" s="12">
+        <f>U8+X7</f>
+        <v>724</v>
+      </c>
+      <c r="Y8" s="16">
+        <f t="shared" si="3"/>
+        <v>724</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="L13"/>
       <c r="M13"/>
@@ -4706,8 +4844,9 @@
       <c r="U13"/>
       <c r="V13"/>
       <c r="W13"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X13"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="L14"/>
       <c r="M14"/>
@@ -4721,8 +4860,9 @@
       <c r="U14"/>
       <c r="V14"/>
       <c r="W14"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X14"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="L15"/>
       <c r="M15"/>
@@ -4736,8 +4876,9 @@
       <c r="U15"/>
       <c r="V15"/>
       <c r="W15"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X15"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="L16"/>
       <c r="M16"/>
@@ -4751,8 +4892,9 @@
       <c r="U16"/>
       <c r="V16"/>
       <c r="W16"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X16"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="L17"/>
       <c r="M17"/>
@@ -4766,8 +4908,9 @@
       <c r="U17"/>
       <c r="V17"/>
       <c r="W17"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X17"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="L18"/>
       <c r="M18"/>
@@ -4781,8 +4924,9 @@
       <c r="U18"/>
       <c r="V18"/>
       <c r="W18"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X18"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="L19"/>
       <c r="M19"/>
@@ -4796,8 +4940,9 @@
       <c r="U19"/>
       <c r="V19"/>
       <c r="W19"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X19"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="L20"/>
       <c r="M20"/>
@@ -4811,8 +4956,9 @@
       <c r="U20"/>
       <c r="V20"/>
       <c r="W20"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X20"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="L21"/>
       <c r="M21"/>
@@ -4826,6 +4972,7 @@
       <c r="U21"/>
       <c r="V21"/>
       <c r="W21"/>
+      <c r="X21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed False 10k & Updated Poster
</commit_message>
<xml_diff>
--- a/Content/WBS.xlsx
+++ b/Content/WBS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\BluSh3ll\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BluSh3ll\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA862DB-1DF3-40C7-ADA6-2CB2D4D0FF93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852F15D2-363A-482A-9999-BFC218C67397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18210" yWindow="1650" windowWidth="19200" windowHeight="17940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
   <si>
     <t>ID</t>
   </si>
@@ -163,18 +163,6 @@
     <t>Have customer deploy product in their enviornment for user testing.</t>
   </si>
   <si>
-    <t>Wk1</t>
-  </si>
-  <si>
-    <t>Wk2</t>
-  </si>
-  <si>
-    <t>Wk3</t>
-  </si>
-  <si>
-    <t>Wk4</t>
-  </si>
-  <si>
     <t>Wk5</t>
   </si>
   <si>
@@ -238,12 +226,6 @@
     <t>Wk23</t>
   </si>
   <si>
-    <t>Wk24</t>
-  </si>
-  <si>
-    <t>Wk25</t>
-  </si>
-  <si>
     <t>Wk26</t>
   </si>
   <si>
@@ -353,6 +335,12 @@
   </si>
   <si>
     <t>Spring Break</t>
+  </si>
+  <si>
+    <t>ID/Week</t>
+  </si>
+  <si>
+    <t>Research</t>
   </si>
 </sst>
 </file>
@@ -451,7 +439,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -507,20 +495,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -532,7 +507,9 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -587,20 +564,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -609,40 +576,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -664,6 +616,23 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -674,6 +643,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,9 +765,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Team Hours'!$B$1:$Y$1</c:f>
+              <c:f>'Team Hours'!$B$1:$X$1</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>Wk5</c:v>
                 </c:pt>
@@ -857,12 +832,9 @@
                   <c:v>Spring Break</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Spring Break</c:v>
+                  <c:v>Wk26</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Wk26</c:v>
-                </c:pt>
-                <c:pt idx="23">
                   <c:v>Wk27</c:v>
                 </c:pt>
               </c:strCache>
@@ -870,10 +842,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Team Hours'!$B$7:$Y$7</c:f>
+              <c:f>'Team Hours'!$B$7:$X$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>11</c:v>
                 </c:pt>
@@ -928,11 +900,11 @@
                 <c:pt idx="19">
                   <c:v>57</c:v>
                 </c:pt>
+                <c:pt idx="21">
+                  <c:v>71</c:v>
+                </c:pt>
                 <c:pt idx="22">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>21</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1193,9 +1165,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Team Hours'!$B$1:$Y$1</c:f>
+              <c:f>'Team Hours'!$B$1:$X$1</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>Wk5</c:v>
                 </c:pt>
@@ -1260,12 +1232,9 @@
                   <c:v>Spring Break</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Spring Break</c:v>
+                  <c:v>Wk26</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Wk26</c:v>
-                </c:pt>
-                <c:pt idx="23">
                   <c:v>Wk27</c:v>
                 </c:pt>
               </c:strCache>
@@ -1273,10 +1242,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Team Hours'!$B$8:$Y$8</c:f>
+              <c:f>'Team Hours'!$B$8:$X$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>11</c:v>
                 </c:pt>
@@ -1304,12 +1273,18 @@
                 <c:pt idx="8">
                   <c:v>288</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>288</c:v>
+                </c:pt>
                 <c:pt idx="10">
                   <c:v>321</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>356</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>356</c:v>
+                </c:pt>
                 <c:pt idx="13">
                   <c:v>389</c:v>
                 </c:pt>
@@ -1331,11 +1306,14 @@
                 <c:pt idx="19">
                   <c:v>653</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>653</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>724</c:v>
+                </c:pt>
                 <c:pt idx="22">
-                  <c:v>724</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>745</c:v>
+                  <c:v>804</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2672,16 +2650,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>386601</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>34739</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>308160</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12327</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>67235</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>145678</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>123266</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2975,7 +2953,7 @@
   <dimension ref="A1:AI18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G11" sqref="A11:G18"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3024,7 +3002,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E2" s="8">
         <v>43703</v>
@@ -3067,7 +3045,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E4" s="9">
         <v>43745</v>
@@ -3090,7 +3068,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E5" s="9">
         <v>43752</v>
@@ -3113,7 +3091,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E6" s="9">
         <v>43759</v>
@@ -3156,7 +3134,7 @@
         <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E8" s="10">
         <v>43766</v>
@@ -3179,7 +3157,7 @@
         <v>33</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E9" s="9">
         <v>43780</v>
@@ -3202,7 +3180,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E10" s="10">
         <v>43794</v>
@@ -3224,8 +3202,8 @@
       <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="46" t="s">
-        <v>77</v>
+      <c r="D11" s="44" t="s">
+        <v>71</v>
       </c>
       <c r="E11" s="9">
         <v>43485</v>
@@ -3247,7 +3225,7 @@
       <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="46"/>
+      <c r="D12" s="44"/>
       <c r="E12" s="10">
         <v>43499</v>
       </c>
@@ -3268,7 +3246,7 @@
       <c r="C13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="46"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="8">
         <v>43513</v>
       </c>
@@ -3289,7 +3267,7 @@
       <c r="C14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="46"/>
+      <c r="D14" s="44"/>
       <c r="E14" s="10">
         <v>43513</v>
       </c>
@@ -3310,7 +3288,7 @@
       <c r="C15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="46"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="10">
         <v>43520</v>
       </c>
@@ -3331,7 +3309,7 @@
       <c r="C16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="46"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="9">
         <v>43526</v>
       </c>
@@ -3352,7 +3330,7 @@
       <c r="C17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="46"/>
+      <c r="D17" s="44"/>
       <c r="E17" s="9">
         <v>43540</v>
       </c>
@@ -3368,12 +3346,12 @@
         <v>4.5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="46"/>
+      <c r="D18" s="44"/>
       <c r="E18" s="10">
         <v>43547</v>
       </c>
@@ -3399,774 +3377,774 @@
   <dimension ref="A1:AC42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:S1048576"/>
+      <selection activeCell="AB18" sqref="AB18:AC18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="5.85546875" customWidth="1"/>
-    <col min="11" max="14" width="5.85546875" style="17" customWidth="1"/>
-    <col min="15" max="15" width="5.85546875" style="34" customWidth="1"/>
-    <col min="16" max="17" width="5.85546875" customWidth="1"/>
-    <col min="18" max="18" width="5.85546875" style="34" customWidth="1"/>
-    <col min="19" max="24" width="5.85546875" customWidth="1"/>
-    <col min="25" max="25" width="5.85546875" style="38" customWidth="1"/>
-    <col min="26" max="29" width="5.85546875" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="9" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="3.7109375" style="41" customWidth="1"/>
+    <col min="11" max="14" width="3.7109375" style="43" customWidth="1"/>
+    <col min="15" max="15" width="3.7109375" style="26" customWidth="1"/>
+    <col min="16" max="17" width="3.7109375" style="41" customWidth="1"/>
+    <col min="18" max="18" width="3.7109375" style="26" customWidth="1"/>
+    <col min="19" max="24" width="3.7109375" style="41" customWidth="1"/>
+    <col min="25" max="25" width="3.7109375" style="29" customWidth="1"/>
+    <col min="26" max="29" width="3.7109375" style="41" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="41" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q1" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="S1" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="T1" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="U1" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="V1" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="W1" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="X1" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y1" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z1" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB1" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC1" s="19" t="s">
+    <row r="1" spans="1:29" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="17">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17">
+        <v>4</v>
+      </c>
+      <c r="F1" s="21">
+        <v>5</v>
+      </c>
+      <c r="G1" s="17">
+        <v>6</v>
+      </c>
+      <c r="H1" s="21">
+        <v>7</v>
+      </c>
+      <c r="I1" s="17">
+        <v>8</v>
+      </c>
+      <c r="J1" s="21">
+        <v>9</v>
+      </c>
+      <c r="K1" s="17">
+        <v>10</v>
+      </c>
+      <c r="L1" s="21">
+        <v>11</v>
+      </c>
+      <c r="M1" s="17">
+        <v>12</v>
+      </c>
+      <c r="N1" s="21">
+        <v>13</v>
+      </c>
+      <c r="O1" s="17">
+        <v>14</v>
+      </c>
+      <c r="P1" s="21">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="17">
+        <v>16</v>
+      </c>
+      <c r="R1" s="18" t="s">
         <v>70</v>
       </c>
+      <c r="S1" s="21">
+        <v>17</v>
+      </c>
+      <c r="T1" s="17">
+        <v>18</v>
+      </c>
+      <c r="U1" s="21">
+        <v>19</v>
+      </c>
+      <c r="V1" s="17">
+        <v>20</v>
+      </c>
+      <c r="W1" s="21">
+        <v>21</v>
+      </c>
+      <c r="X1" s="17">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="21">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="17">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="21">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="17">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="21">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="19">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="18"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
+      <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="49" t="s">
-        <v>18</v>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="47" t="s">
+        <v>101</v>
       </c>
       <c r="I3" s="50"/>
       <c r="J3" s="50"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="18"/>
-      <c r="AA3" s="18"/>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="18"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="40"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="40"/>
+      <c r="AA3" s="40"/>
+      <c r="AB3" s="40"/>
+      <c r="AC3" s="40"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
+      <c r="A4" s="19">
         <v>2.1</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="24">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="20">
         <v>2.1</v>
       </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z4" s="18"/>
-      <c r="AA4" s="18"/>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="18"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+      <c r="Y4" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="40"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="A5" s="19">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="24">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="20">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z5" s="18"/>
-      <c r="AA5" s="18"/>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="18"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
+      <c r="X5" s="40"/>
+      <c r="Y5" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z5" s="40"/>
+      <c r="AA5" s="40"/>
+      <c r="AB5" s="40"/>
+      <c r="AC5" s="40"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="31">
+      <c r="A6" s="23">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="24">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="20">
         <v>2.2999999999999998</v>
       </c>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z6" s="18"/>
-      <c r="AA6" s="18"/>
-      <c r="AB6" s="18"/>
-      <c r="AC6" s="18"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+      <c r="X6" s="40"/>
+      <c r="Y6" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z6" s="40"/>
+      <c r="AA6" s="40"/>
+      <c r="AB6" s="40"/>
+      <c r="AC6" s="40"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="17">
         <v>3</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="49" t="s">
-        <v>78</v>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="47" t="s">
+        <v>72</v>
       </c>
       <c r="L7" s="50"/>
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
-      <c r="O7" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="P7" s="49" t="s">
+      <c r="O7" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="P7" s="47" t="s">
         <v>5</v>
       </c>
       <c r="Q7" s="50"/>
-      <c r="R7" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S7" s="49" t="s">
-        <v>80</v>
+      <c r="R7" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="S7" s="47" t="s">
+        <v>74</v>
       </c>
       <c r="T7" s="50"/>
       <c r="U7" s="50"/>
       <c r="V7" s="50"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
-      <c r="AB7" s="18"/>
-      <c r="AC7" s="18"/>
+      <c r="W7" s="40"/>
+      <c r="X7" s="40"/>
+      <c r="Y7" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z7" s="40"/>
+      <c r="AA7" s="40"/>
+      <c r="AB7" s="40"/>
+      <c r="AC7" s="40"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
+      <c r="A8" s="19">
         <v>3.1</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="47">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="45">
         <v>3.1</v>
       </c>
-      <c r="L8" s="48"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="18"/>
-      <c r="Y8" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z8" s="18"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="18"/>
-      <c r="AC8" s="18"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="S8" s="40"/>
+      <c r="T8" s="40"/>
+      <c r="U8" s="40"/>
+      <c r="V8" s="40"/>
+      <c r="W8" s="40"/>
+      <c r="X8" s="40"/>
+      <c r="Y8" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z8" s="40"/>
+      <c r="AA8" s="40"/>
+      <c r="AB8" s="40"/>
+      <c r="AC8" s="40"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="23">
+      <c r="A9" s="19">
         <v>3.2</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="47">
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="45">
         <v>3.2</v>
       </c>
-      <c r="N9" s="48"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="Z9" s="18"/>
-      <c r="AA9" s="18"/>
-      <c r="AB9" s="18"/>
-      <c r="AC9" s="18"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
+      <c r="V9" s="40"/>
+      <c r="W9" s="40"/>
+      <c r="X9" s="40"/>
+      <c r="Y9" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z9" s="40"/>
+      <c r="AA9" s="40"/>
+      <c r="AB9" s="40"/>
+      <c r="AC9" s="40"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
+      <c r="A10" s="19">
         <v>3.3</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="P10" s="47">
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="P10" s="45">
         <v>3.3</v>
       </c>
-      <c r="Q10" s="48"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="37"/>
-      <c r="Z10" s="18"/>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="18"/>
-      <c r="AC10" s="18"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="40"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="40"/>
+      <c r="W10" s="40"/>
+      <c r="X10" s="40"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="40"/>
+      <c r="AA10" s="40"/>
+      <c r="AB10" s="40"/>
+      <c r="AC10" s="40"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
+      <c r="A11" s="19">
         <v>3.4</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="S11" s="47">
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="S11" s="45">
         <v>3.4</v>
       </c>
-      <c r="T11" s="48"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
-      <c r="AC11" s="18"/>
+      <c r="T11" s="46"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="40"/>
+      <c r="W11" s="40"/>
+      <c r="X11" s="40"/>
+      <c r="Y11" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z11" s="40"/>
+      <c r="AA11" s="40"/>
+      <c r="AB11" s="40"/>
+      <c r="AC11" s="40"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="23">
+      <c r="A12" s="19">
         <v>3.5</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="S12" s="40"/>
+      <c r="T12" s="40"/>
       <c r="U12" s="51">
         <v>3.5</v>
       </c>
       <c r="V12" s="52"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z12" s="18"/>
-      <c r="AA12" s="18"/>
-      <c r="AB12" s="18"/>
-      <c r="AC12" s="18"/>
+      <c r="W12" s="40"/>
+      <c r="X12" s="40"/>
+      <c r="Y12" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z12" s="40"/>
+      <c r="AA12" s="40"/>
+      <c r="AB12" s="40"/>
+      <c r="AC12" s="40"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+      <c r="A13" s="17">
         <v>4</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="49" t="s">
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="47" t="s">
         <v>7</v>
       </c>
       <c r="X13" s="50"/>
-      <c r="Y13" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z13" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA13" s="49"/>
-      <c r="AB13" s="49"/>
-      <c r="AC13" s="49"/>
+      <c r="Y13" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z13" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA13" s="47"/>
+      <c r="AB13" s="47"/>
+      <c r="AC13" s="47"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="23">
+      <c r="A14" s="19">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="24">
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="40"/>
+      <c r="W14" s="20">
         <v>4.0999999999999996</v>
       </c>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z14" s="18"/>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-      <c r="AC14" s="18"/>
+      <c r="X14" s="42"/>
+      <c r="Y14" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z14" s="40"/>
+      <c r="AA14" s="40"/>
+      <c r="AB14" s="40"/>
+      <c r="AC14" s="40"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="23">
+      <c r="A15" s="19">
         <v>4.2</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="36">
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="40"/>
+      <c r="W15" s="40"/>
+      <c r="X15" s="38">
         <v>4.2</v>
       </c>
-      <c r="Y15" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z15" s="18"/>
-      <c r="AA15" s="18"/>
-      <c r="AB15" s="18"/>
-      <c r="AC15" s="18"/>
+      <c r="Y15" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z15" s="40"/>
+      <c r="AA15" s="40"/>
+      <c r="AB15" s="40"/>
+      <c r="AC15" s="40"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="23">
+      <c r="A16" s="19">
         <v>4.3</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="37"/>
-      <c r="Z16" s="27">
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="40"/>
+      <c r="T16" s="40"/>
+      <c r="U16" s="40"/>
+      <c r="V16" s="40"/>
+      <c r="W16" s="40"/>
+      <c r="X16" s="40"/>
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="37">
         <v>4.2</v>
       </c>
-      <c r="AA16" s="18"/>
-      <c r="AB16" s="18"/>
-      <c r="AC16" s="18"/>
+      <c r="AA16" s="40"/>
+      <c r="AB16" s="40"/>
+      <c r="AC16" s="40"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="23">
+      <c r="A17" s="19">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-      <c r="X17" s="18"/>
-      <c r="Y17" s="37"/>
-      <c r="Z17" s="18"/>
-      <c r="AA17" s="24">
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="40"/>
+      <c r="W17" s="40"/>
+      <c r="X17" s="40"/>
+      <c r="Y17" s="28"/>
+      <c r="Z17" s="40"/>
+      <c r="AA17" s="20">
         <v>4.4000000000000004</v>
       </c>
-      <c r="AB17" s="18"/>
-      <c r="AC17" s="18"/>
+      <c r="AB17" s="40"/>
+      <c r="AC17" s="40"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="23">
+      <c r="A18" s="19">
         <v>4.5</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="37"/>
-      <c r="Z18" s="18"/>
-      <c r="AA18" s="18"/>
-      <c r="AB18" s="47">
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="40"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="40"/>
+      <c r="W18" s="40"/>
+      <c r="X18" s="40"/>
+      <c r="Y18" s="28"/>
+      <c r="Z18" s="40"/>
+      <c r="AA18" s="40"/>
+      <c r="AB18" s="45">
         <v>4.5</v>
       </c>
-      <c r="AC18" s="48"/>
+      <c r="AC18" s="46"/>
     </row>
     <row r="19" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:29" hidden="1" x14ac:dyDescent="0.25"/>
@@ -4214,10 +4192,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C261B442-2F63-4F7C-A433-D2B145AB0897}">
-  <dimension ref="A1:Z21"/>
+  <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:Y6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD25" sqref="AD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4226,91 +4204,90 @@
     <col min="2" max="2" width="5.85546875" style="11" customWidth="1"/>
     <col min="3" max="3" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="13" width="5.85546875" style="11" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" style="39" bestFit="1" customWidth="1"/>
-    <col min="15" max="24" width="5.85546875" style="11" customWidth="1"/>
-    <col min="25" max="25" width="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="21" width="5.85546875" style="11" customWidth="1"/>
+    <col min="22" max="22" width="12" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.85546875" style="11" customWidth="1"/>
+    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="42" t="s">
+      <c r="M1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="N1" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="O1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="U1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="V1" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="W1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="U1" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="V1" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="W1" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z1" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y1" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B2" s="14">
         <v>4</v>
@@ -4339,14 +4316,14 @@
       <c r="J2" s="14">
         <v>8</v>
       </c>
-      <c r="K2" s="43"/>
+      <c r="K2" s="34"/>
       <c r="L2" s="11">
         <v>7</v>
       </c>
       <c r="M2" s="11">
         <v>8</v>
       </c>
-      <c r="N2" s="41"/>
+      <c r="N2" s="32"/>
       <c r="O2" s="11">
         <v>7</v>
       </c>
@@ -4368,20 +4345,21 @@
       <c r="U2" s="11">
         <v>14</v>
       </c>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="11">
+      <c r="V2" s="36"/>
+      <c r="W2" s="11">
         <v>15</v>
       </c>
-      <c r="Y2" s="16"/>
-      <c r="Z2">
-        <f t="shared" ref="Z2:Z7" si="0">AVERAGE(B2:X2)</f>
-        <v>8.1578947368421044</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X2" s="16">
+        <v>17</v>
+      </c>
+      <c r="Y2">
+        <f>AVERAGE(B2:X2)</f>
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B3" s="14">
         <v>3</v>
@@ -4410,14 +4388,14 @@
       <c r="J3" s="14">
         <v>8</v>
       </c>
-      <c r="K3" s="43"/>
+      <c r="K3" s="34"/>
       <c r="L3" s="11">
         <v>6</v>
       </c>
       <c r="M3" s="11">
         <v>7</v>
       </c>
-      <c r="N3" s="41"/>
+      <c r="N3" s="32"/>
       <c r="O3" s="11">
         <v>6</v>
       </c>
@@ -4439,20 +4417,21 @@
       <c r="U3" s="11">
         <v>11</v>
       </c>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="11">
+      <c r="V3" s="36"/>
+      <c r="W3" s="11">
         <v>14</v>
       </c>
-      <c r="Y3" s="16"/>
-      <c r="Z3">
-        <f t="shared" si="0"/>
-        <v>7.0526315789473681</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X3" s="16">
+        <v>15</v>
+      </c>
+      <c r="Y3">
+        <f>AVERAGE(B3:X3)</f>
+        <v>7.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B4" s="14">
         <v>2</v>
@@ -4481,14 +4460,14 @@
       <c r="J4" s="14">
         <v>7</v>
       </c>
-      <c r="K4" s="43"/>
+      <c r="K4" s="34"/>
       <c r="L4" s="11">
         <v>6</v>
       </c>
       <c r="M4" s="11">
         <v>6</v>
       </c>
-      <c r="N4" s="41"/>
+      <c r="N4" s="32"/>
       <c r="O4" s="11">
         <v>6</v>
       </c>
@@ -4510,20 +4489,21 @@
       <c r="U4" s="11">
         <v>9</v>
       </c>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="11">
+      <c r="V4" s="36"/>
+      <c r="W4" s="11">
         <v>14</v>
       </c>
-      <c r="Y4" s="16"/>
-      <c r="Z4">
-        <f t="shared" si="0"/>
-        <v>7.1578947368421053</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X4" s="16">
+        <v>14</v>
+      </c>
+      <c r="Y4">
+        <f>AVERAGE(B4:X4)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B5" s="14">
         <v>1</v>
@@ -4552,14 +4532,14 @@
       <c r="J5" s="14">
         <v>8</v>
       </c>
-      <c r="K5" s="43"/>
+      <c r="K5" s="34"/>
       <c r="L5" s="11">
         <v>7</v>
       </c>
       <c r="M5" s="11">
         <v>6</v>
       </c>
-      <c r="N5" s="41"/>
+      <c r="N5" s="32"/>
       <c r="O5" s="11">
         <v>7</v>
       </c>
@@ -4581,20 +4561,21 @@
       <c r="U5" s="11">
         <v>11</v>
       </c>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="11">
+      <c r="V5" s="36"/>
+      <c r="W5" s="11">
         <v>12</v>
       </c>
-      <c r="Y5" s="16"/>
-      <c r="Z5">
-        <f t="shared" si="0"/>
-        <v>7.1052631578947372</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X5" s="16">
+        <v>13</v>
+      </c>
+      <c r="Y5">
+        <f>AVERAGE(B5:X5)</f>
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B6" s="14">
         <v>1</v>
@@ -4623,14 +4604,14 @@
       <c r="J6" s="14">
         <v>9</v>
       </c>
-      <c r="K6" s="43"/>
+      <c r="K6" s="34"/>
       <c r="L6" s="11">
         <v>7</v>
       </c>
       <c r="M6" s="11">
         <v>8</v>
       </c>
-      <c r="N6" s="41"/>
+      <c r="N6" s="32"/>
       <c r="O6" s="11">
         <v>7</v>
       </c>
@@ -4652,115 +4633,113 @@
       <c r="U6" s="11">
         <v>12</v>
       </c>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
-      <c r="X6" s="11">
+      <c r="V6" s="36"/>
+      <c r="W6" s="11">
         <v>16</v>
       </c>
-      <c r="Y6" s="16">
+      <c r="X6" s="16">
         <v>21</v>
       </c>
-      <c r="Z6">
-        <f>AVERAGE(B6:Y6)</f>
+      <c r="Y6">
+        <f>AVERAGE(B6:X6)</f>
         <v>9.25</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B7" s="14">
-        <f t="shared" ref="B7:Y7" si="1">SUM(B2:B6)</f>
+        <f t="shared" ref="B7:X7" si="0">SUM(B2:B6)</f>
         <v>11</v>
       </c>
       <c r="C7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="D7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="E7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="F7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="G7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="H7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="I7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="J7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="K7" s="43"/>
+      <c r="K7" s="34"/>
       <c r="L7" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="M7" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="N7" s="41"/>
+      <c r="N7" s="32"/>
       <c r="O7" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="P7" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="Q7" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="R7" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="S7" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="T7" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="U7" s="39">
-        <f t="shared" ref="U7" si="2">SUM(U2:U6)</f>
+      <c r="U7" s="30">
+        <f t="shared" ref="U7" si="1">SUM(U2:U6)</f>
         <v>57</v>
       </c>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
+      <c r="V7" s="36"/>
+      <c r="W7" s="16">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
       <c r="X7" s="16">
-        <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="Y7" s="16">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="Z7">
         <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="Y7">
+        <f>AVERAGE(B7:W7)</f>
         <v>38.10526315789474</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B8" s="11">
         <f>B7</f>
@@ -4771,83 +4750,91 @@
         <v>52</v>
       </c>
       <c r="D8" s="12">
-        <f t="shared" ref="D8:Y8" si="3">C8+D7</f>
+        <f t="shared" ref="D8:X8" si="2">C8+D7</f>
         <v>93</v>
       </c>
       <c r="E8" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>124</v>
       </c>
       <c r="F8" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>154</v>
       </c>
       <c r="G8" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>187</v>
       </c>
       <c r="H8" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>220</v>
       </c>
       <c r="I8" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>248</v>
       </c>
       <c r="J8" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>288</v>
       </c>
-      <c r="K8" s="43"/>
+      <c r="K8" s="39">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
       <c r="L8" s="12">
         <f>J8+L7</f>
         <v>321</v>
       </c>
       <c r="M8" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>356</v>
       </c>
-      <c r="N8" s="41"/>
+      <c r="N8" s="39">
+        <f t="shared" si="2"/>
+        <v>356</v>
+      </c>
       <c r="O8" s="12">
         <f>M8+O7</f>
         <v>389</v>
       </c>
       <c r="P8" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>424</v>
       </c>
       <c r="Q8" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>462</v>
       </c>
       <c r="R8" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>501</v>
       </c>
       <c r="S8" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>537</v>
       </c>
       <c r="T8" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>596</v>
       </c>
-      <c r="U8" s="39">
-        <f t="shared" si="3"/>
+      <c r="U8" s="30">
+        <f t="shared" si="2"/>
         <v>653</v>
       </c>
-      <c r="V8" s="45"/>
-      <c r="W8" s="45"/>
-      <c r="X8" s="12">
-        <f>U8+X7</f>
+      <c r="V8" s="39">
+        <f t="shared" si="2"/>
+        <v>653</v>
+      </c>
+      <c r="W8" s="12">
+        <f>U8+W7</f>
         <v>724</v>
       </c>
-      <c r="Y8" s="16">
-        <f t="shared" si="3"/>
-        <v>745</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X8" s="16">
+        <f t="shared" si="2"/>
+        <v>804</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="L13"/>
       <c r="M13"/>
@@ -4861,9 +4848,8 @@
       <c r="U13"/>
       <c r="V13"/>
       <c r="W13"/>
-      <c r="X13"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="L14"/>
       <c r="M14"/>
@@ -4877,9 +4863,8 @@
       <c r="U14"/>
       <c r="V14"/>
       <c r="W14"/>
-      <c r="X14"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="L15"/>
       <c r="M15"/>
@@ -4893,9 +4878,8 @@
       <c r="U15"/>
       <c r="V15"/>
       <c r="W15"/>
-      <c r="X15"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="L16"/>
       <c r="M16"/>
@@ -4909,9 +4893,8 @@
       <c r="U16"/>
       <c r="V16"/>
       <c r="W16"/>
-      <c r="X16"/>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="L17"/>
       <c r="M17"/>
@@ -4925,9 +4908,8 @@
       <c r="U17"/>
       <c r="V17"/>
       <c r="W17"/>
-      <c r="X17"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="L18"/>
       <c r="M18"/>
@@ -4941,9 +4923,8 @@
       <c r="U18"/>
       <c r="V18"/>
       <c r="W18"/>
-      <c r="X18"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="L19"/>
       <c r="M19"/>
@@ -4957,9 +4938,8 @@
       <c r="U19"/>
       <c r="V19"/>
       <c r="W19"/>
-      <c r="X19"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="L20"/>
       <c r="M20"/>
@@ -4973,9 +4953,8 @@
       <c r="U20"/>
       <c r="V20"/>
       <c r="W20"/>
-      <c r="X20"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="L21"/>
       <c r="M21"/>
@@ -4989,7 +4968,6 @@
       <c r="U21"/>
       <c r="V21"/>
       <c r="W21"/>
-      <c r="X21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>